<commit_message>
Incorporated the gen_landmark function
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Documents\MAE 7560 Optimal Estimation for Aerospace\Course Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\pburton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9B16C5-17C3-4441-830F-D253E73CFCDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44C0D8-4BF1-451E-A7DD-AA2C0A9DD83B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,22 +32,11 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="250">
   <si>
     <t>Value</t>
   </si>
@@ -476,24 +465,6 @@
   </si>
   <si>
     <t>alpha</t>
-  </si>
-  <si>
-    <t>thx_st</t>
-  </si>
-  <si>
-    <t>thy_st</t>
-  </si>
-  <si>
-    <t>thz_st</t>
-  </si>
-  <si>
-    <t>z angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
-    <t>y angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
-  </si>
-  <si>
-    <t>x angle of a ZYX euler angle sequence to define ST orientation wrt body</t>
   </si>
   <si>
     <t>thz_c</t>
@@ -1419,23 +1390,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
@@ -1452,7 +1423,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>6</v>
       </c>
@@ -1470,7 +1441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1488,7 +1459,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>41</v>
       </c>
@@ -1506,7 +1477,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1496,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1543,7 +1514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>58</v>
       </c>
@@ -1561,7 +1532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>129</v>
       </c>
@@ -1580,7 +1551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>43</v>
       </c>
@@ -1598,7 +1569,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>44</v>
       </c>
@@ -1616,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>45</v>
       </c>
@@ -1634,7 +1605,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>46</v>
       </c>
@@ -1652,7 +1623,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>47</v>
       </c>
@@ -1670,7 +1641,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>48</v>
       </c>
@@ -1688,7 +1659,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>123</v>
       </c>
@@ -1706,7 +1677,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>49</v>
       </c>
@@ -1724,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>50</v>
       </c>
@@ -1742,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>51</v>
       </c>
@@ -1760,9 +1731,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B19" s="66">
         <f>$B$5/2</f>
@@ -1772,16 +1743,16 @@
         <v>5</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E19" s="63">
         <f t="shared" ref="E19:E20" si="1">B19</f>
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B20" s="66">
         <f>$B$5/2</f>
@@ -1798,7 +1769,7 @@
         <v>3404.7101009954345</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>35</v>
       </c>
@@ -1816,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>20</v>
       </c>
@@ -1834,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>37</v>
       </c>
@@ -1852,9 +1823,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B24" s="62">
         <v>0</v>
@@ -1866,16 +1837,16 @@
         <v>146</v>
       </c>
       <c r="E24" s="63">
-        <f t="shared" ref="E24:E29" si="3">RADIANS(B24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" ref="E24:E26" si="3">RADIANS(B24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>144</v>
       </c>
       <c r="B25" s="62">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>22</v>
@@ -1885,15 +1856,15 @@
       </c>
       <c r="E25" s="63">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B26" s="62">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>22</v>
@@ -1903,528 +1874,474 @@
       </c>
       <c r="E26" s="63">
         <f t="shared" si="3"/>
-        <v>3.1415926535897931</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.52359877559829882</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B27" s="62">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E27" s="63">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" ref="E27:E28" si="4">B27</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B28" s="62">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E28" s="63">
-        <f t="shared" si="3"/>
-        <v>0.17453292519943295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B29" s="62">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E29" s="63">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <f>B29/1000</f>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B30" s="62">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E30" s="63">
-        <f t="shared" ref="E30:E31" si="4">B30</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <f>B30*0.000001</f>
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B31" s="62">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E31" s="63">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" ref="E31:E32" si="5">B31</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B32" s="62">
-        <v>19</v>
+        <v>2500</v>
       </c>
       <c r="C32" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>167</v>
-      </c>
       <c r="E32" s="63">
-        <f>B32/1000</f>
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B33" s="62">
-        <v>7</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E33" s="63">
-        <f>B33*0.000001</f>
-        <v>6.9999999999999999E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="62">
-        <v>2500</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E34" s="63">
-        <f t="shared" ref="E34:E35" si="5">B34</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="B35" s="62">
-        <v>2500</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="63">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="64">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="64">
         <v>5</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="63">
-        <f>B36</f>
+      <c r="D33" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="63">
+        <f>B33</f>
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="49">
+      <c r="B34" s="49">
         <v>1</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C34" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D34" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="51">
-        <f t="shared" ref="E37:E39" si="6">B37</f>
+      <c r="E34" s="51">
+        <f t="shared" ref="E34:E36" si="6">B34</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="52" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="53">
+      <c r="B35" s="53">
         <v>1</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="C35" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D35" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="E38" s="55">
+      <c r="E35" s="55">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="B39" s="69">
-        <v>0</v>
-      </c>
-      <c r="C39" s="47" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="B36" s="69">
+        <v>0</v>
+      </c>
+      <c r="C36" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="E39" s="61">
+      <c r="D36" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="61">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="64">
+        <v>0</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="63">
+        <f t="shared" ref="E37" si="7">B37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="67">
+        <v>0</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="68">
+        <f t="shared" ref="E38:E51" si="8">B38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1737.5</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="1">
+        <f>B39*1000</f>
+        <v>1737500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B40" s="64">
-        <v>0</v>
+        <v>221</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1737.5</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="E40" s="63">
-        <f t="shared" ref="E40" si="7">B40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="67">
-        <v>0</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="68">
-        <f t="shared" ref="E41:E54" si="8">B41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+      <c r="E40" s="1">
+        <f>B40*1000</f>
+        <v>1737500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="8"/>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B42" s="2">
-        <v>1737.5</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="16" t="s">
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="E42" s="1">
-        <f>B42*1000</f>
-        <v>1737500</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1737.5</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" s="1">
-        <f>B43*1000</f>
-        <v>1737500</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
-        <v>229</v>
-      </c>
       <c r="B44" s="2">
         <v>0</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B45" s="2">
-        <v>1.62</v>
+        <v>-1</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="8"/>
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
+      <c r="C46" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B46" s="2">
-        <v>0</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>236</v>
-      </c>
       <c r="D46" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B47" s="2">
         <v>0</v>
       </c>
       <c r="C47" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="1">
+        <f>B47*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1738</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" ref="E48:E49" si="9">B48*1000</f>
+        <v>1738000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="D47" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="B48" s="2">
-        <v>-1</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="1">
-        <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
-        <v>234</v>
-      </c>
       <c r="B49" s="2">
         <v>0</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>237</v>
+        <v>53</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>240</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>53</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>241</v>
+      </c>
+      <c r="B50" s="84">
+        <v>2.7E-6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>243</v>
       </c>
       <c r="D50" s="16" t="s">
         <v>244</v>
       </c>
       <c r="E50" s="1">
-        <f>B50*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1738</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" ref="E51:E52" si="9">B51*1000</f>
-        <v>1738000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="E52" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>247</v>
-      </c>
-      <c r="B53" s="84">
-        <v>2.7E-6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>249</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="E53" s="1">
         <f t="shared" si="8"/>
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>248</v>
-      </c>
-      <c r="B54" s="85">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" s="85">
         <v>4904869500000</v>
       </c>
-      <c r="C54" t="s">
-        <v>251</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E54" s="1">
+      <c r="C51" t="s">
+        <v>245</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51" s="1">
         <f t="shared" si="8"/>
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>253</v>
-      </c>
-      <c r="B55" s="2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>247</v>
+      </c>
+      <c r="B52" s="2">
         <v>1737.5</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C52" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="E55" s="1">
-        <f>B55*1000</f>
+      <c r="D52" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="E52" s="1">
+        <f>B52*1000</f>
         <v>1737500</v>
       </c>
     </row>
@@ -2442,13 +2359,13 @@
       <selection activeCell="B7" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2464,7 +2381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2473,7 +2390,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2481,9 +2398,9 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -2500,18 +2417,18 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="84" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2528,7 +2445,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>72</v>
       </c>
@@ -2546,7 +2463,7 @@
         <v>-390000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>74</v>
       </c>
@@ -2565,7 +2482,7 @@
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>76</v>
       </c>
@@ -2583,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>78</v>
       </c>
@@ -2601,7 +2518,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>80</v>
       </c>
@@ -2619,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>81</v>
       </c>
@@ -2637,9 +2554,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B8" s="45">
         <v>0</v>
@@ -2648,16 +2565,16 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E8" s="80">
         <f>B8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B9" s="29">
         <v>0</v>
@@ -2666,16 +2583,16 @@
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E9" s="80">
         <f t="shared" ref="E9:E19" si="1">B9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B10" s="70">
         <v>0</v>
@@ -2684,16 +2601,16 @@
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E10" s="80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="71" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -2702,16 +2619,16 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E11" s="81">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -2720,16 +2637,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E12" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B13" s="70">
         <v>0</v>
@@ -2738,16 +2655,16 @@
         <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E13" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B14" s="70">
         <v>0</v>
@@ -2756,16 +2673,16 @@
         <v>0</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="71" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -2774,16 +2691,16 @@
         <v>0</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E15" s="28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B16" s="76">
         <v>0</v>
@@ -2792,16 +2709,16 @@
         <v>53</v>
       </c>
       <c r="D16" s="76" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E16" s="83">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -2810,16 +2727,16 @@
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E17" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B18" s="16">
         <v>0</v>
@@ -2828,16 +2745,16 @@
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E18" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="71" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B19" s="8">
         <v>0</v>
@@ -2846,16 +2763,16 @@
         <v>0</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E19" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="75" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B20" s="76">
         <v>0</v>
@@ -2864,16 +2781,16 @@
         <v>53</v>
       </c>
       <c r="D20" s="76" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E20" s="82">
         <f>B20*1000</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -2882,16 +2799,16 @@
         <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E21" s="82">
         <f>B21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B22" s="16">
         <v>0</v>
@@ -2900,16 +2817,16 @@
         <v>0</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E22" s="82">
         <f t="shared" ref="E22:E23" si="2">B22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="71" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B23" s="8">
         <v>0</v>
@@ -2918,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E23" s="82">
         <f t="shared" si="2"/>
@@ -2939,14 +2856,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2963,7 +2880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2980,7 +2897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2997,7 +2914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3014,9 +2931,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3031,9 +2948,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -3048,7 +2965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -3065,9 +2982,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -3082,9 +2999,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -3099,7 +3016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3116,7 +3033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3146,14 +3063,14 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3170,7 +3087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3187,7 +3104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3204,9 +3121,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3221,7 +3138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -3238,9 +3155,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -3255,9 +3172,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -3272,7 +3189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -3291,7 +3208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3321,17 +3238,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -3348,7 +3265,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>130</v>
       </c>
@@ -3367,7 +3284,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3386,7 +3303,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3404,7 +3321,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>103</v>
       </c>
@@ -3422,7 +3339,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>104</v>
       </c>
@@ -3440,7 +3357,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>105</v>
       </c>
@@ -3458,7 +3375,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>106</v>
       </c>
@@ -3476,7 +3393,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3494,7 +3411,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>136</v>
       </c>
@@ -3512,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>137</v>
       </c>
@@ -3530,9 +3447,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B12" s="9">
         <v>10</v>
@@ -3541,16 +3458,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E12" s="1">
         <f>B12/3</f>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B13" s="9">
         <v>100</v>
@@ -3559,16 +3476,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E13" s="1">
         <f>B13/3</f>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B14" s="9">
         <v>10</v>
@@ -3577,7 +3494,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E14" s="1">
         <f>B14/3</f>
@@ -3598,17 +3515,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3625,7 +3542,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -3643,7 +3560,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -3661,7 +3578,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
@@ -3679,7 +3596,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -3697,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>94</v>
       </c>
@@ -3715,7 +3632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
@@ -3733,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>108</v>
       </c>
@@ -3751,7 +3668,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>109</v>
       </c>
@@ -3769,7 +3686,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>110</v>
       </c>
@@ -3787,7 +3704,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>114</v>
       </c>
@@ -3806,7 +3723,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>115</v>
       </c>
@@ -3825,7 +3742,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>116</v>
       </c>
@@ -3844,7 +3761,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>111</v>
       </c>
@@ -3863,7 +3780,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>112</v>
       </c>
@@ -3882,7 +3799,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>113</v>
       </c>
@@ -3901,7 +3818,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -3920,7 +3837,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
@@ -3939,7 +3856,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>102</v>
       </c>
@@ -3970,18 +3887,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -3998,7 +3915,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -4021,7 +3938,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -4044,7 +3961,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -4067,7 +3984,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4090,7 +4007,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4112,7 +4029,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4134,7 +4051,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4156,7 +4073,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4178,7 +4095,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4200,7 +4117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4222,7 +4139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4244,7 +4161,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4266,7 +4183,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4302,17 +4219,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -4329,7 +4246,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4352,7 +4269,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4375,7 +4292,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4398,7 +4315,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4421,7 +4338,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4443,7 +4360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4465,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4487,7 +4404,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4509,7 +4426,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4531,7 +4448,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4553,7 +4470,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4575,7 +4492,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4597,7 +4514,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4619,7 +4536,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4641,7 +4558,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4663,7 +4580,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4685,7 +4602,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4707,7 +4624,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4743,16 +4660,16 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.77734375" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -4769,7 +4686,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>117</v>
       </c>
@@ -4789,7 +4706,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>118</v>
       </c>
@@ -4809,7 +4726,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>119</v>
       </c>
@@ -4829,7 +4746,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
@@ -4849,7 +4766,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -4869,7 +4786,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>122</v>
       </c>
@@ -4896,9 +4813,9 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B8" s="6">
         <v>10</v>
@@ -4907,7 +4824,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E8" s="72">
         <f>B8</f>
@@ -4922,16 +4839,16 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E9" s="72">
         <f t="shared" ref="E9:E15" si="1">B9</f>
@@ -4946,16 +4863,16 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B10" s="6">
         <v>2</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E10" s="72">
         <f t="shared" si="1"/>
@@ -4970,16 +4887,16 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E11" s="72">
         <f t="shared" si="1"/>
@@ -4994,9 +4911,9 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B12" s="16">
         <v>10</v>
@@ -5005,7 +4922,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E12" s="72">
         <f t="shared" si="1"/>
@@ -5020,16 +4937,16 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B13" s="16">
         <v>1</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="16" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E13" s="72">
         <f t="shared" si="1"/>
@@ -5044,16 +4961,16 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B14" s="16">
         <v>1</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="16" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E14" s="72">
         <f t="shared" si="1"/>
@@ -5068,16 +4985,16 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B15" s="17">
         <v>1</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E15" s="73">
         <f t="shared" si="1"/>
@@ -5092,7 +5009,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5107,7 +5024,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5122,7 +5039,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5137,7 +5054,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5152,7 +5069,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5167,7 +5084,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>

</xml_diff>

<commit_message>
Added error state propogation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\pburton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Burton_MAE7560\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44C0D8-4BF1-451E-A7DD-AA2C0A9DD83B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3874E1-3DC3-4FC0-A97A-6B94AEEE2517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,22 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="253">
   <si>
     <t>Value</t>
   </si>
@@ -786,6 +797,15 @@
   </si>
   <si>
     <t>tau_a</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>m/s3</t>
+  </si>
+  <si>
+    <t>m/s4</t>
   </si>
 </sst>
 </file>
@@ -798,7 +818,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,6 +837,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1392,21 +1418,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
@@ -1423,7 +1449,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
         <v>6</v>
       </c>
@@ -1441,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1459,7 +1485,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>41</v>
       </c>
@@ -1477,7 +1503,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>42</v>
       </c>
@@ -1496,7 +1522,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1514,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>58</v>
       </c>
@@ -1532,7 +1558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>129</v>
       </c>
@@ -1551,7 +1577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>43</v>
       </c>
@@ -1569,7 +1595,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>44</v>
       </c>
@@ -1587,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>45</v>
       </c>
@@ -1605,7 +1631,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>46</v>
       </c>
@@ -1623,7 +1649,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>47</v>
       </c>
@@ -1641,7 +1667,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>48</v>
       </c>
@@ -1659,7 +1685,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>123</v>
       </c>
@@ -1677,7 +1703,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>49</v>
       </c>
@@ -1695,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>50</v>
       </c>
@@ -1713,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>51</v>
       </c>
@@ -1731,13 +1757,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>217</v>
       </c>
       <c r="B19" s="66">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
+        <v>55</v>
       </c>
       <c r="C19" s="65" t="s">
         <v>5</v>
@@ -1747,16 +1772,15 @@
       </c>
       <c r="E19" s="63">
         <f t="shared" ref="E19:E20" si="1">B19</f>
-        <v>3404.7101009954345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>249</v>
       </c>
       <c r="B20" s="66">
-        <f>$B$5/2</f>
-        <v>3404.7101009954345</v>
+        <v>55</v>
       </c>
       <c r="C20" s="65" t="s">
         <v>5</v>
@@ -1766,10 +1790,10 @@
       </c>
       <c r="E20" s="63">
         <f t="shared" si="1"/>
-        <v>3404.7101009954345</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>35</v>
       </c>
@@ -1787,12 +1811,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>4</v>
@@ -1802,10 +1826,10 @@
       </c>
       <c r="E22" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>37</v>
       </c>
@@ -1823,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>143</v>
       </c>
@@ -1841,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>144</v>
       </c>
@@ -1859,7 +1883,7 @@
         <v>-1.5707963267948966</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>145</v>
       </c>
@@ -1877,7 +1901,7 @@
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>140</v>
       </c>
@@ -1895,7 +1919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>142</v>
       </c>
@@ -1913,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>156</v>
       </c>
@@ -1931,7 +1955,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>167</v>
       </c>
@@ -1949,7 +1973,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>159</v>
       </c>
@@ -1967,7 +1991,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>160</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>168</v>
       </c>
@@ -2003,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="48" t="s">
         <v>125</v>
       </c>
@@ -2021,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="52" t="s">
         <v>126</v>
       </c>
@@ -2039,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
         <v>171</v>
       </c>
@@ -2057,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>172</v>
       </c>
@@ -2075,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>174</v>
       </c>
@@ -2093,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>219</v>
       </c>
@@ -2111,7 +2135,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>221</v>
       </c>
@@ -2129,7 +2153,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>223</v>
       </c>
@@ -2147,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>224</v>
       </c>
@@ -2165,7 +2189,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>225</v>
       </c>
@@ -2183,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>226</v>
       </c>
@@ -2201,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>227</v>
       </c>
@@ -2219,7 +2243,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="18" t="s">
         <v>228</v>
       </c>
@@ -2237,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
         <v>229</v>
       </c>
@@ -2255,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>236</v>
       </c>
@@ -2273,7 +2297,7 @@
         <v>1738000</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>237</v>
       </c>
@@ -2291,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>241</v>
       </c>
@@ -2309,7 +2333,7 @@
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>242</v>
       </c>
@@ -2327,7 +2351,7 @@
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>247</v>
       </c>
@@ -2359,13 +2383,13 @@
       <selection activeCell="B7" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2373,7 +2397,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2381,7 +2405,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2390,7 +2414,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2398,7 +2422,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -2420,15 +2444,15 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="84" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2445,7 +2469,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>72</v>
       </c>
@@ -2463,7 +2487,7 @@
         <v>-390000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>74</v>
       </c>
@@ -2482,7 +2506,7 @@
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>76</v>
       </c>
@@ -2500,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>78</v>
       </c>
@@ -2518,7 +2542,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>80</v>
       </c>
@@ -2536,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>81</v>
       </c>
@@ -2554,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
         <v>176</v>
       </c>
@@ -2572,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>177</v>
       </c>
@@ -2590,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
         <v>178</v>
       </c>
@@ -2608,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="71" t="s">
         <v>179</v>
       </c>
@@ -2626,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="74" t="s">
         <v>197</v>
       </c>
@@ -2644,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
         <v>198</v>
       </c>
@@ -2662,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="36" t="s">
         <v>199</v>
       </c>
@@ -2680,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
         <v>200</v>
       </c>
@@ -2698,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
         <v>201</v>
       </c>
@@ -2716,7 +2740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="74" t="s">
         <v>202</v>
       </c>
@@ -2734,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
         <v>203</v>
       </c>
@@ -2752,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="71" t="s">
         <v>204</v>
       </c>
@@ -2770,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="75" t="s">
         <v>205</v>
       </c>
@@ -2788,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="74" t="s">
         <v>206</v>
       </c>
@@ -2806,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>207</v>
       </c>
@@ -2824,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
         <v>208</v>
       </c>
@@ -2856,14 +2880,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2880,7 +2904,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2897,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2914,7 +2938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2931,7 +2955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2948,7 +2972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -2965,7 +2989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2982,7 +3006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>183</v>
       </c>
@@ -2999,7 +3023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -3016,7 +3040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3033,7 +3057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3060,17 +3084,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3087,7 +3111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3104,7 +3128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3121,7 +3145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -3138,7 +3162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -3155,7 +3179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -3172,7 +3196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -3189,7 +3213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -3208,7 +3232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3238,17 +3262,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -3265,7 +3289,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>130</v>
       </c>
@@ -3284,7 +3308,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -3303,7 +3327,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -3321,7 +3345,7 @@
         <v>4.8481368110953598E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>103</v>
       </c>
@@ -3339,7 +3363,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>104</v>
       </c>
@@ -3357,7 +3381,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>105</v>
       </c>
@@ -3375,7 +3399,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>106</v>
       </c>
@@ -3393,7 +3417,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3411,7 +3435,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>136</v>
       </c>
@@ -3429,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>137</v>
       </c>
@@ -3447,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>149</v>
       </c>
@@ -3465,7 +3489,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>151</v>
       </c>
@@ -3483,7 +3507,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>153</v>
       </c>
@@ -3515,17 +3539,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3542,7 +3566,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -3560,7 +3584,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -3578,7 +3602,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
@@ -3596,7 +3620,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -3614,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>94</v>
       </c>
@@ -3632,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>95</v>
       </c>
@@ -3650,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>108</v>
       </c>
@@ -3668,7 +3692,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>109</v>
       </c>
@@ -3686,7 +3710,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>110</v>
       </c>
@@ -3704,7 +3728,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>114</v>
       </c>
@@ -3723,7 +3747,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>115</v>
       </c>
@@ -3742,7 +3766,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>116</v>
       </c>
@@ -3761,7 +3785,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>111</v>
       </c>
@@ -3780,7 +3804,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>112</v>
       </c>
@@ -3799,7 +3823,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>113</v>
       </c>
@@ -3818,7 +3842,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -3837,7 +3861,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
@@ -3856,7 +3880,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>102</v>
       </c>
@@ -3887,18 +3911,18 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -3915,7 +3939,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="str">
         <f>truthStateParams!A2</f>
         <v>Q_grav</v>
@@ -3938,7 +3962,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
@@ -3961,7 +3985,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>truthStateParams!A4</f>
         <v>arw</v>
@@ -3984,7 +4008,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_st_ss</v>
@@ -4007,7 +4031,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_c_ss</v>
@@ -4029,7 +4053,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_meas_stx</v>
@@ -4051,7 +4075,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_meas_sty</v>
@@ -4073,7 +4097,7 @@
         <v>2.4240684055476799E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="str">
         <f>truthStateParams!A9</f>
         <v>sig_meas_stz</v>
@@ -4095,7 +4119,7 @@
         <v>1.4544410433286079E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="str">
         <f>truthStateParams!A10</f>
         <v>sig_cu</v>
@@ -4117,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="str">
         <f>truthStateParams!A11</f>
         <v>sig_cv</v>
@@ -4139,7 +4163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_idpos</v>
@@ -4161,7 +4185,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_loss</v>
@@ -4183,7 +4207,7 @@
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_mdpos</v>
@@ -4219,17 +4243,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="51.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -4246,7 +4270,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
@@ -4269,7 +4293,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
@@ -4292,7 +4316,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
@@ -4315,7 +4339,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
@@ -4338,7 +4362,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
@@ -4360,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
@@ -4382,7 +4406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
@@ -4404,7 +4428,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
@@ -4426,7 +4450,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
@@ -4448,7 +4472,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
@@ -4470,7 +4494,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
@@ -4492,7 +4516,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
@@ -4514,7 +4538,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
@@ -4536,7 +4560,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
@@ -4558,7 +4582,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
@@ -4580,7 +4604,7 @@
         <v>3.2320912073969067E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
@@ -4602,7 +4626,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="str">
         <f>truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
@@ -4624,7 +4648,7 @@
         <v>8.0802280184922667E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f>truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
@@ -4657,19 +4681,20 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
@@ -4686,7 +4711,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>117</v>
       </c>
@@ -4706,7 +4731,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>118</v>
       </c>
@@ -4726,7 +4751,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>119</v>
       </c>
@@ -4746,7 +4771,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
@@ -4766,7 +4791,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>121</v>
       </c>
@@ -4786,7 +4811,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>122</v>
       </c>
@@ -4813,7 +4838,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>185</v>
       </c>
@@ -4839,20 +4864,22 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6"/>
+      <c r="B9" s="26">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>230</v>
+      </c>
       <c r="D9" s="6" t="s">
         <v>190</v>
       </c>
       <c r="E9" s="72">
         <f t="shared" ref="E9:E15" si="1">B9</f>
-        <v>1</v>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="F9" s="6"/>
       <c r="I9" s="6"/>
@@ -4863,20 +4890,22 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="26">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>190</v>
       </c>
       <c r="E10" s="72">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F10" s="6"/>
       <c r="I10" s="6"/>
@@ -4887,20 +4916,22 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="6">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6"/>
+      <c r="B11" s="26">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="D11" s="6" t="s">
         <v>190</v>
       </c>
       <c r="E11" s="72">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="F11" s="6"/>
       <c r="I11" s="6"/>
@@ -4911,12 +4942,12 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>191</v>
       </c>
       <c r="B12" s="16">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>8</v>
@@ -4926,7 +4957,7 @@
       </c>
       <c r="E12" s="72">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F12" s="6"/>
       <c r="I12" s="6"/>
@@ -4937,20 +4968,22 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>193</v>
       </c>
       <c r="B13" s="16">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="D13" s="16" t="s">
         <v>196</v>
       </c>
       <c r="E13" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.2699999999999999E-3</v>
       </c>
       <c r="F13" s="6"/>
       <c r="I13" s="6"/>
@@ -4961,20 +4994,22 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>194</v>
       </c>
       <c r="B14" s="16">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6"/>
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="D14" s="16" t="s">
         <v>196</v>
       </c>
       <c r="E14" s="72">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.2699999999999999E-3</v>
       </c>
       <c r="F14" s="6"/>
       <c r="I14" s="6"/>
@@ -4985,20 +5020,22 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>250</v>
+      </c>
       <c r="D15" s="17" t="s">
         <v>196</v>
       </c>
       <c r="E15" s="73">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3.2699999999999999E-3</v>
       </c>
       <c r="F15" s="6"/>
       <c r="I15" s="6"/>
@@ -5009,7 +5046,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5024,7 +5061,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5039,7 +5076,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5054,7 +5091,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5069,7 +5106,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5084,7 +5121,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5100,6 +5137,7 @@
       <c r="O21" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Documentation for errorProp
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Burton_MAE7560\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3874E1-3DC3-4FC0-A97A-6B94AEEE2517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF20F0C6-E769-4E55-A2C0-17EAD78306A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -1418,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2440,7 +2440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Linear Measurement Model
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Burton_MAE7560\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF20F0C6-E769-4E55-A2C0-17EAD78306A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424CD406-FE6A-42BE-9A45-ED96F2D382CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1798,7 @@
         <v>35</v>
       </c>
       <c r="B21" s="64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>4</v>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="E21" s="63">
         <f t="shared" ref="E21:E23" si="2">B21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1834,7 +1834,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>4</v>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="E23" s="63">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2440,7 +2440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
@@ -4680,7 +4680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed values in spreadsheet documented B matrix
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Burton_MAE7560\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\pburton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623E0BE-3840-424A-9C2E-236E0ECAE601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438A08F-DCE0-4DE3-9093-AEF9EC7DE0DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="894" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,22 +32,11 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="232">
   <si>
     <t>Value</t>
   </si>
@@ -737,6 +726,12 @@
   </si>
   <si>
     <t>sig_vx</t>
+  </si>
+  <si>
+    <t>m/s/sqrt(hr)</t>
+  </si>
+  <si>
+    <t>3-sigma accelerometer velocity random walk</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1090,6 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1438,17 +1434,17 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1461,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
@@ -1483,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -1501,7 +1497,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>34</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
@@ -1538,7 +1534,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>51</v>
       </c>
@@ -1574,7 +1570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>85</v>
       </c>
@@ -1593,7 +1589,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>36</v>
       </c>
@@ -1611,7 +1607,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>37</v>
       </c>
@@ -1629,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>38</v>
       </c>
@@ -1647,7 +1643,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>39</v>
       </c>
@@ -1665,7 +1661,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>40</v>
       </c>
@@ -1683,7 +1679,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>41</v>
       </c>
@@ -1701,7 +1697,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>80</v>
       </c>
@@ -1719,7 +1715,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1755,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>161</v>
       </c>
@@ -1791,7 +1787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>193</v>
       </c>
@@ -1809,7 +1805,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
@@ -1827,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>93</v>
       </c>
@@ -1881,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>94</v>
       </c>
@@ -1899,7 +1895,7 @@
         <v>-1.5707963267948966</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>95</v>
       </c>
@@ -1917,7 +1913,7 @@
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>90</v>
       </c>
@@ -1935,7 +1931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>92</v>
       </c>
@@ -1953,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>100</v>
       </c>
@@ -1971,7 +1967,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>111</v>
       </c>
@@ -1989,7 +1985,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>103</v>
       </c>
@@ -2007,7 +2003,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>104</v>
       </c>
@@ -2025,7 +2021,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>112</v>
       </c>
@@ -2043,7 +2039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>82</v>
       </c>
@@ -2061,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>115</v>
       </c>
@@ -2079,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>116</v>
       </c>
@@ -2097,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>118</v>
       </c>
@@ -2115,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>163</v>
       </c>
@@ -2133,7 +2129,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>165</v>
       </c>
@@ -2151,7 +2147,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>167</v>
       </c>
@@ -2169,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>168</v>
       </c>
@@ -2187,7 +2183,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>169</v>
       </c>
@@ -2205,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>170</v>
       </c>
@@ -2223,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>171</v>
       </c>
@@ -2241,7 +2237,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>172</v>
       </c>
@@ -2259,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>173</v>
       </c>
@@ -2277,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>180</v>
       </c>
@@ -2295,7 +2291,7 @@
         <v>1738000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>181</v>
       </c>
@@ -2313,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>185</v>
       </c>
@@ -2331,7 +2327,7 @@
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>186</v>
       </c>
@@ -2349,7 +2345,7 @@
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>191</v>
       </c>
@@ -2378,16 +2374,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A6:B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +2391,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2403,7 +2399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2412,7 +2408,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2439,18 +2435,18 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
@@ -2467,7 +2463,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>64</v>
       </c>
@@ -2485,7 +2481,7 @@
         <v>-390000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>66</v>
       </c>
@@ -2504,7 +2500,7 @@
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>68</v>
       </c>
@@ -2522,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>70</v>
       </c>
@@ -2540,7 +2536,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>72</v>
       </c>
@@ -2558,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>73</v>
       </c>
@@ -2576,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>120</v>
       </c>
@@ -2594,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>121</v>
       </c>
@@ -2612,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>122</v>
       </c>
@@ -2630,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
         <v>123</v>
       </c>
@@ -2648,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>141</v>
       </c>
@@ -2666,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>142</v>
       </c>
@@ -2684,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>143</v>
       </c>
@@ -2702,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
         <v>144</v>
       </c>
@@ -2720,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
         <v>145</v>
       </c>
@@ -2738,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
         <v>146</v>
       </c>
@@ -2756,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>147</v>
       </c>
@@ -2774,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>148</v>
       </c>
@@ -2792,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="61" t="s">
         <v>149</v>
       </c>
@@ -2810,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>150</v>
       </c>
@@ -2828,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>151</v>
       </c>
@@ -2846,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>152</v>
       </c>
@@ -2878,14 +2874,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2902,7 +2898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2919,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2936,7 +2932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2953,7 +2949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -2970,7 +2966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -2987,7 +2983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -3004,7 +3000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -3021,7 +3017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -3038,7 +3034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -3055,7 +3051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3081,18 +3077,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD82E9-FB96-4FE4-9B12-1EDF4DE7082A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3109,7 +3105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3126,7 +3122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3143,7 +3139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -3160,7 +3156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -3177,7 +3173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3194,7 +3190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3211,7 +3207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3230,7 +3226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3258,21 +3254,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -3289,7 +3285,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>218</v>
       </c>
@@ -3308,87 +3304,102 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>219</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>225</v>
       </c>
       <c r="E3" s="10">
-        <v>1</v>
+        <f>B3/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>220</v>
       </c>
       <c r="B4" s="10">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>194</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>226</v>
       </c>
       <c r="E4" s="10">
-        <v>2</v>
+        <f>B4/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="10">
-        <v>3</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="B5" s="83">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>227</v>
       </c>
       <c r="E5" s="10">
-        <v>3</v>
+        <f>B5/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>222</v>
       </c>
       <c r="B6" s="10">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="D6" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E6" s="10">
-        <v>4</v>
+        <f>B6/3</f>
+        <v>16.666666666666668</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>223</v>
       </c>
       <c r="B7" s="10">
-        <v>3.3330000000000002E-4</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
-        <v>224</v>
+        <v>0.06</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>231</v>
       </c>
       <c r="E7" s="10">
-        <v>3.3330000000000002E-4</v>
+        <f>B7/SQRT(hr2sec)/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="9"/>
       <c r="C8" s="13"/>
@@ -3396,7 +3407,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="9"/>
       <c r="C9" s="13"/>
@@ -3404,7 +3415,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -3412,7 +3423,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -3420,7 +3431,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -3428,7 +3439,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -3436,7 +3447,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -3455,21 +3466,21 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E15" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
@@ -3486,7 +3497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>212</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>213</v>
       </c>
@@ -3522,7 +3533,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>214</v>
       </c>
@@ -3540,7 +3551,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>229</v>
       </c>
@@ -3558,7 +3569,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>216</v>
       </c>
@@ -3576,7 +3587,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>215</v>
       </c>
@@ -3594,12 +3605,13 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>197</v>
       </c>
       <c r="B8" s="13">
-        <v>10</v>
+        <f>truthStateParams!B3</f>
+        <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -3609,14 +3621,15 @@
       </c>
       <c r="E8" s="78">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>198</v>
       </c>
       <c r="B9" s="19">
+        <f>truthStateParams!B5</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -3630,11 +3643,12 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
         <v>199</v>
       </c>
       <c r="B10" s="19">
+        <f>truthStateParams!B5</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -3648,11 +3662,12 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>200</v>
       </c>
       <c r="B11" s="19">
+        <f>truthStateParams!B5</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -3666,11 +3681,12 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>201</v>
       </c>
       <c r="B12" s="72">
+        <f>truthStateParams!B6</f>
         <v>50</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -3684,11 +3700,12 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>202</v>
       </c>
       <c r="B13" s="5">
+        <f>truthStateParams!$B$4</f>
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3698,14 +3715,16 @@
         <v>209</v>
       </c>
       <c r="E13" s="78">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <f>B13/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>203</v>
       </c>
       <c r="B14" s="5">
+        <f>truthStateParams!$B$4</f>
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3715,14 +3734,16 @@
         <v>209</v>
       </c>
       <c r="E14" s="78">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>B14/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="79" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="80">
+      <c r="B15" s="5">
+        <f>truthStateParams!$B$4</f>
         <v>1</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -3731,21 +3752,22 @@
       <c r="D15" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="E15" s="81">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="78">
+        <f>B15/1000/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="19"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="19"/>
     </row>
   </sheetData>
@@ -3762,18 +3784,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -3790,12 +3812,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B2" s="19">
-        <f>0.00000016*3</f>
+        <f>truthStateParams!B2</f>
         <v>4.8000000000000006E-7</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -3805,16 +3827,17 @@
         <v>87</v>
       </c>
       <c r="E2" s="11">
-        <f>truthStateParams!E2</f>
+        <f>B2/3</f>
         <v>1.6000000000000003E-7</v>
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="19">
+        <f>truthStateParams!B3</f>
         <v>1</v>
       </c>
       <c r="C3" s="19"/>
@@ -3822,109 +3845,113 @@
         <v>225</v>
       </c>
       <c r="E3" s="11">
-        <f>truthStateParams!E3</f>
-        <v>1</v>
+        <f>B3/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="10">
-        <v>2</v>
+      <c r="B4" s="19">
+        <f>truthStateParams!B4</f>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>226</v>
       </c>
       <c r="E4" s="11">
-        <f>truthStateParams!E4</f>
-        <v>2</v>
+        <f>B4/1000/3</f>
+        <v>3.3333333333333332E-4</v>
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="10">
-        <v>3</v>
+      <c r="B5" s="19">
+        <f>truthStateParams!B5</f>
+        <v>6.0000000000000002E-5</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="5" t="s">
         <v>227</v>
       </c>
       <c r="E5" s="11">
-        <f>truthStateParams!E5</f>
-        <v>3</v>
+        <f>B5/3</f>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="10">
-        <v>4</v>
+      <c r="B6" s="19">
+        <f>truthStateParams!B6</f>
+        <v>50</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E6" s="11">
-        <f>truthStateParams!E6</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <f>B6/3</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B7" s="10">
-        <v>3.3330000000000002E-4</v>
+      <c r="B7" s="19">
+        <f>truthStateParams!B7</f>
+        <v>0.06</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
         <v>224</v>
       </c>
       <c r="E7" s="11">
-        <f>truthStateParams!E7</f>
-        <v>3.3330000000000002E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <f>B7/SQRT(hr2sec)/3</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="9"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="9"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -3940,21 +3967,21 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E2" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
@@ -3971,11 +3998,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>212</v>
       </c>
       <c r="B2" s="5">
+        <f>truthStateInitialUncertainty!B2</f>
         <v>400</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -3985,16 +4013,16 @@
         <v>210</v>
       </c>
       <c r="E2" s="78">
-        <f t="shared" ref="E2:E12" si="0">B2/3</f>
         <v>133.33333333333334</v>
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="5">
+        <f>truthStateInitialUncertainty!B3</f>
         <v>400</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -4004,16 +4032,16 @@
         <v>210</v>
       </c>
       <c r="E3" s="78">
-        <f t="shared" si="0"/>
         <v>133.33333333333334</v>
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>214</v>
       </c>
       <c r="B4" s="5">
+        <f>truthStateInitialUncertainty!B4</f>
         <v>400</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -4023,16 +4051,16 @@
         <v>210</v>
       </c>
       <c r="E4" s="78">
-        <f t="shared" si="0"/>
         <v>133.33333333333334</v>
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>229</v>
       </c>
       <c r="B5" s="5">
+        <f>truthStateInitialUncertainty!B5</f>
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -4042,16 +4070,16 @@
         <v>211</v>
       </c>
       <c r="E5" s="78">
-        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>216</v>
       </c>
       <c r="B6" s="5">
+        <f>truthStateInitialUncertainty!B6</f>
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -4061,15 +4089,15 @@
         <v>211</v>
       </c>
       <c r="E6" s="78">
-        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>215</v>
       </c>
       <c r="B7" s="5">
+        <f>truthStateInitialUncertainty!B7</f>
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -4079,16 +4107,16 @@
         <v>211</v>
       </c>
       <c r="E7" s="78">
-        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="13">
-        <v>10</v>
+      <c r="B8" s="5">
+        <f>truthStateInitialUncertainty!B8</f>
+        <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -4097,15 +4125,15 @@
         <v>207</v>
       </c>
       <c r="E8" s="78">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="5">
+        <f>truthStateInitialUncertainty!B9</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -4115,15 +4143,15 @@
         <v>206</v>
       </c>
       <c r="E9" s="78">
-        <f t="shared" si="0"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
         <v>199</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="5">
+        <f>truthStateInitialUncertainty!B10</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -4133,15 +4161,15 @@
         <v>206</v>
       </c>
       <c r="E10" s="78">
-        <f t="shared" si="0"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="5">
+        <f>truthStateInitialUncertainty!B11</f>
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -4151,15 +4179,15 @@
         <v>206</v>
       </c>
       <c r="E11" s="78">
-        <f t="shared" si="0"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>201</v>
       </c>
-      <c r="B12" s="72">
+      <c r="B12" s="5">
+        <f>truthStateInitialUncertainty!B12</f>
         <v>50</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -4169,15 +4197,15 @@
         <v>208</v>
       </c>
       <c r="E12" s="78">
-        <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>202</v>
       </c>
       <c r="B13" s="5">
+        <f>truthStateInitialUncertainty!B13</f>
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4187,14 +4215,15 @@
         <v>209</v>
       </c>
       <c r="E13" s="78">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>203</v>
       </c>
       <c r="B14" s="5">
+        <f>truthStateInitialUncertainty!B14</f>
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4204,14 +4233,15 @@
         <v>209</v>
       </c>
       <c r="E14" s="78">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="79" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="80">
+      <c r="B15" s="5">
+        <f>truthStateInitialUncertainty!B15</f>
         <v>1</v>
       </c>
       <c r="C15" s="80" t="s">
@@ -4221,19 +4251,19 @@
         <v>209</v>
       </c>
       <c r="E15" s="81">
-        <v>3.2699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3.3333333333333332E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
     </row>
   </sheetData>
@@ -4251,17 +4281,17 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -4278,7 +4308,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -4298,7 +4328,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
@@ -4318,7 +4348,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>76</v>
       </c>
@@ -4338,7 +4368,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
@@ -4358,7 +4388,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>78</v>
       </c>
@@ -4378,7 +4408,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>79</v>
       </c>
@@ -4405,7 +4435,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>129</v>
       </c>
@@ -4431,7 +4461,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>131</v>
       </c>
@@ -4457,7 +4487,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>132</v>
       </c>
@@ -4483,7 +4513,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>133</v>
       </c>
@@ -4509,7 +4539,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>135</v>
       </c>
@@ -4535,7 +4565,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>137</v>
       </c>
@@ -4561,7 +4591,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>138</v>
       </c>
@@ -4587,7 +4617,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>139</v>
       </c>
@@ -4613,7 +4643,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -4628,7 +4658,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4643,7 +4673,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4658,7 +4688,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4673,7 +4703,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4688,7 +4718,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>

</xml_diff>

<commit_message>
Generalized the calc_attitude function
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porte\Burton_MAE7560\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rchristensen\repos\student_repos\pburton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3719EB7E-BC4B-46A9-A0CD-CFB2A3DB4968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973827D1-E91A-426C-808A-EC9A3443BE67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="894" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -32,17 +32,6 @@
     <definedName name="min2sec">Constants!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1437,21 +1426,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1457,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -1504,7 +1493,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>34</v>
       </c>
@@ -1522,7 +1511,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
@@ -1541,7 +1530,7 @@
         <v>6809.4202019908689</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>51</v>
       </c>
@@ -1577,13 +1566,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="50">
-        <f>12*6</f>
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>4</v>
@@ -1593,10 +1581,10 @@
       </c>
       <c r="E8" s="49">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>36</v>
       </c>
@@ -1614,7 +1602,7 @@
         <v>4902801076000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>37</v>
       </c>
@@ -1632,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>38</v>
       </c>
@@ -1650,7 +1638,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>39</v>
       </c>
@@ -1668,7 +1656,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>40</v>
       </c>
@@ -1686,7 +1674,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>41</v>
       </c>
@@ -1704,7 +1692,7 @@
         <v>1737400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>80</v>
       </c>
@@ -1722,7 +1710,7 @@
         <v>2.6616994576329732E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
@@ -1740,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>43</v>
       </c>
@@ -1758,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>44</v>
       </c>
@@ -1776,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>161</v>
       </c>
@@ -1794,7 +1782,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>193</v>
       </c>
@@ -1812,7 +1800,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
@@ -1830,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -1848,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>30</v>
       </c>
@@ -1866,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>93</v>
       </c>
@@ -1884,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>94</v>
       </c>
@@ -1902,7 +1890,7 @@
         <v>-1.5707963267948966</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>95</v>
       </c>
@@ -1920,7 +1908,7 @@
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>90</v>
       </c>
@@ -1938,7 +1926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>92</v>
       </c>
@@ -1956,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>100</v>
       </c>
@@ -1974,7 +1962,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>111</v>
       </c>
@@ -1992,7 +1980,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>103</v>
       </c>
@@ -2010,7 +1998,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>104</v>
       </c>
@@ -2028,7 +2016,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>112</v>
       </c>
@@ -2046,7 +2034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38" t="s">
         <v>82</v>
       </c>
@@ -2064,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>115</v>
       </c>
@@ -2082,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>116</v>
       </c>
@@ -2100,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>118</v>
       </c>
@@ -2118,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>163</v>
       </c>
@@ -2136,7 +2124,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>165</v>
       </c>
@@ -2154,7 +2142,7 @@
         <v>1737500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>167</v>
       </c>
@@ -2172,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>168</v>
       </c>
@@ -2190,7 +2178,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>169</v>
       </c>
@@ -2208,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>170</v>
       </c>
@@ -2226,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>171</v>
       </c>
@@ -2244,7 +2232,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>172</v>
       </c>
@@ -2262,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>173</v>
       </c>
@@ -2280,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>180</v>
       </c>
@@ -2298,7 +2286,7 @@
         <v>1738000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>181</v>
       </c>
@@ -2316,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>185</v>
       </c>
@@ -2334,7 +2322,7 @@
         <v>2.7E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>186</v>
       </c>
@@ -2352,7 +2340,7 @@
         <v>4904869500000</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>191</v>
       </c>
@@ -2384,13 +2372,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2398,7 +2386,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2406,7 +2394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2415,7 +2403,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2423,7 +2411,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2441,19 +2429,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D12A37-CB3D-4FDB-95C9-F32EFDA07C44}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
@@ -2470,7 +2458,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>64</v>
       </c>
@@ -2488,7 +2476,7 @@
         <v>-390000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>66</v>
       </c>
@@ -2507,7 +2495,7 @@
         <v>1747895.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>68</v>
       </c>
@@ -2525,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>70</v>
       </c>
@@ -2543,7 +2531,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>72</v>
       </c>
@@ -2561,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>73</v>
       </c>
@@ -2579,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>120</v>
       </c>
@@ -2597,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>121</v>
       </c>
@@ -2615,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>122</v>
       </c>
@@ -2633,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
         <v>123</v>
       </c>
@@ -2651,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>141</v>
       </c>
@@ -2669,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>142</v>
       </c>
@@ -2687,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>143</v>
       </c>
@@ -2705,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
         <v>144</v>
       </c>
@@ -2723,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="61" t="s">
         <v>145</v>
       </c>
@@ -2741,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
         <v>146</v>
       </c>
@@ -2759,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>147</v>
       </c>
@@ -2777,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>148</v>
       </c>
@@ -2795,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="61" t="s">
         <v>149</v>
       </c>
@@ -2813,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>150</v>
       </c>
@@ -2831,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>151</v>
       </c>
@@ -2849,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>152</v>
       </c>
@@ -2878,17 +2866,17 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2905,7 +2893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2922,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2939,7 +2927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2956,7 +2944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -2973,7 +2961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>126</v>
       </c>
@@ -2990,7 +2978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -3007,7 +2995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -3024,7 +3012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -3041,7 +3029,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -3058,7 +3046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3085,17 +3073,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3112,7 +3100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3129,7 +3117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3146,7 +3134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -3163,7 +3151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -3180,7 +3168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -3197,7 +3185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -3214,7 +3202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3233,7 +3221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3265,17 +3253,17 @@
       <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -3292,7 +3280,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>218</v>
       </c>
@@ -3311,7 +3299,7 @@
         <v>1.6000000000000003E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>219</v>
       </c>
@@ -3330,7 +3318,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>220</v>
       </c>
@@ -3349,7 +3337,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>221</v>
       </c>
@@ -3368,7 +3356,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>222</v>
       </c>
@@ -3387,7 +3375,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>223</v>
       </c>
@@ -3406,7 +3394,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="9"/>
       <c r="C8" s="13"/>
@@ -3414,7 +3402,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="9"/>
       <c r="C9" s="13"/>
@@ -3422,7 +3410,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -3430,7 +3418,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -3438,7 +3426,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -3446,7 +3434,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -3454,7 +3442,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -3476,18 +3464,18 @@
       <selection activeCell="E15" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3492,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>212</v>
       </c>
@@ -3522,7 +3510,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>213</v>
       </c>
@@ -3540,7 +3528,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>214</v>
       </c>
@@ -3558,7 +3546,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>229</v>
       </c>
@@ -3576,7 +3564,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>216</v>
       </c>
@@ -3594,7 +3582,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>215</v>
       </c>
@@ -3612,7 +3600,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>197</v>
       </c>
@@ -3631,7 +3619,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>198</v>
       </c>
@@ -3650,7 +3638,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
         <v>199</v>
       </c>
@@ -3669,7 +3657,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>200</v>
       </c>
@@ -3688,7 +3676,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>201</v>
       </c>
@@ -3707,7 +3695,7 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>202</v>
       </c>
@@ -3726,7 +3714,7 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>203</v>
       </c>
@@ -3745,7 +3733,7 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="79" t="s">
         <v>204</v>
       </c>
@@ -3764,17 +3752,17 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="19"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="19"/>
     </row>
   </sheetData>
@@ -3791,18 +3779,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -3819,7 +3807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>218</v>
       </c>
@@ -3839,7 +3827,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>219</v>
       </c>
@@ -3857,7 +3845,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>220</v>
       </c>
@@ -3874,7 +3862,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>221</v>
       </c>
@@ -3892,7 +3880,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>222</v>
       </c>
@@ -3909,7 +3897,7 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>223</v>
       </c>
@@ -3926,39 +3914,39 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="9"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="9"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -3977,18 +3965,18 @@
       <selection activeCell="E2" sqref="E2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="5"/>
+    <col min="4" max="4" width="51.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
@@ -4005,7 +3993,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>212</v>
       </c>
@@ -4024,7 +4012,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>213</v>
       </c>
@@ -4043,7 +4031,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>214</v>
       </c>
@@ -4062,7 +4050,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>229</v>
       </c>
@@ -4081,7 +4069,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>216</v>
       </c>
@@ -4099,7 +4087,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>215</v>
       </c>
@@ -4117,7 +4105,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>197</v>
       </c>
@@ -4135,7 +4123,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>198</v>
       </c>
@@ -4153,7 +4141,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
         <v>199</v>
       </c>
@@ -4171,7 +4159,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>200</v>
       </c>
@@ -4189,7 +4177,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>201</v>
       </c>
@@ -4207,7 +4195,7 @@
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>202</v>
       </c>
@@ -4225,7 +4213,7 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>203</v>
       </c>
@@ -4243,7 +4231,7 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="79" t="s">
         <v>204</v>
       </c>
@@ -4261,16 +4249,16 @@
         <v>3.3333333333333332E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
     </row>
   </sheetData>
@@ -4288,17 +4276,17 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -4315,7 +4303,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -4335,7 +4323,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
@@ -4355,7 +4343,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>76</v>
       </c>
@@ -4375,7 +4363,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
@@ -4395,7 +4383,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>78</v>
       </c>
@@ -4415,7 +4403,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>79</v>
       </c>
@@ -4442,7 +4430,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>129</v>
       </c>
@@ -4468,7 +4456,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>131</v>
       </c>
@@ -4494,7 +4482,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>132</v>
       </c>
@@ -4520,7 +4508,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>133</v>
       </c>
@@ -4546,7 +4534,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>135</v>
       </c>
@@ -4572,7 +4560,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>137</v>
       </c>
@@ -4598,7 +4586,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>138</v>
       </c>
@@ -4624,7 +4612,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>139</v>
       </c>
@@ -4650,7 +4638,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -4665,7 +4653,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4680,7 +4668,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -4695,7 +4683,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -4710,7 +4698,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -4725,7 +4713,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>

</xml_diff>